<commit_message>
data and figure update
</commit_message>
<xml_diff>
--- a/data/timelines_data_v3.xlsx
+++ b/data/timelines_data_v3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ucbtds4\R_Repositories\rodent_borne_zoonoses\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBE1166-476E-41E7-9CA0-D57FED179E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B155FA-2144-4767-AA6A-3D6E9091367E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7164" yWindow="2844" windowWidth="17280" windowHeight="9996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="206">
   <si>
     <t>disease</t>
   </si>
@@ -488,15 +488,6 @@
     <t>Mus baoulei as hosts</t>
   </si>
   <si>
-    <t>Hantavirus Pulmonary Syndrome</t>
-  </si>
-  <si>
-    <t>United States of America</t>
-  </si>
-  <si>
-    <t>Identified as cause of unrecognised cases</t>
-  </si>
-  <si>
     <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC1869168/pdf/amjpathol00051-0009.pdf</t>
   </si>
   <si>
@@ -506,9 +497,6 @@
     <t>https://www.cdc.gov/mmwr/preview/mmwrhtml/00020769.htm</t>
   </si>
   <si>
-    <t>Virus isolated and cultured</t>
-  </si>
-  <si>
     <t>Hantavirus Pulmonary Syndrome described</t>
   </si>
   <si>
@@ -621,6 +609,51 @@
   </si>
   <si>
     <t>https://doi.org/10.1371/journal.pntd.0006968</t>
+  </si>
+  <si>
+    <t>Haemorrhagic Fever with Renal Syndrome/Hantavirus Pulmonary Syndrome</t>
+  </si>
+  <si>
+    <t>SNV Identified as cause of unrecognised cases</t>
+  </si>
+  <si>
+    <t>SNV isolated and cultured</t>
+  </si>
+  <si>
+    <t>Puumala virus as cause of Nephropathia Epidemica</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1093/infdis/141.2.131</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1002/jmv.1890380211</t>
+  </si>
+  <si>
+    <t>Dobrova virus identified</t>
+  </si>
+  <si>
+    <t>Saaremaa virus identified</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/S0140-6736(05)63206-0</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1006/viro.1996.0305</t>
+  </si>
+  <si>
+    <t>Andes virus identified</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1093%2Finfdis%2F146.5.638</t>
+  </si>
+  <si>
+    <t>Hantaan virus identified</t>
+  </si>
+  <si>
+    <t>Seoul virus identified</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3904/kjim.1989.4.2.130</t>
   </si>
 </sst>
 </file>
@@ -962,10 +995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F100"/>
+  <dimension ref="A1:F106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2286,10 +2319,10 @@
         <v>33</v>
       </c>
       <c r="E66" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -2306,7 +2339,7 @@
         <v>33</v>
       </c>
       <c r="E67" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F67" s="3"/>
     </row>
@@ -2532,433 +2565,553 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="B79" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="C79">
-        <v>1983</v>
+        <v>-6000</v>
       </c>
       <c r="D79" t="s">
         <v>5</v>
       </c>
       <c r="E79" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="B80" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="C80">
-        <v>1993</v>
+        <v>-1500</v>
       </c>
       <c r="D80" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E80" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="B81" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="C81">
-        <v>1993</v>
+        <v>-400</v>
       </c>
       <c r="D81" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E81" t="s">
-        <v>156</v>
+        <v>173</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="B82" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="C82">
-        <v>1993</v>
+        <v>1920</v>
       </c>
       <c r="D82" t="s">
         <v>10</v>
       </c>
       <c r="E82" t="s">
-        <v>157</v>
+        <v>175</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="B83" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="C83">
-        <v>2011</v>
+        <v>1972</v>
       </c>
       <c r="D83" t="s">
         <v>10</v>
       </c>
       <c r="E83" t="s">
-        <v>158</v>
+        <v>24</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="B84" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="C84">
-        <v>1993</v>
+        <v>1977</v>
       </c>
       <c r="D84" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E84" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>161</v>
+        <v>179</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="B85" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="C85">
-        <v>1995</v>
+        <v>1851</v>
       </c>
       <c r="D85" t="s">
         <v>11</v>
       </c>
       <c r="E85" t="s">
-        <v>162</v>
-      </c>
-      <c r="F85" s="3" t="s">
-        <v>163</v>
+        <v>180</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="B86" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="C86">
-        <v>1993</v>
+        <v>1859</v>
       </c>
       <c r="D86" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="E86" t="s">
-        <v>164</v>
-      </c>
-      <c r="F86" s="3" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="B87" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="C87">
-        <v>2021</v>
+        <v>1915</v>
       </c>
       <c r="D87" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="E87" t="s">
-        <v>166</v>
-      </c>
-      <c r="F87" s="3" t="s">
-        <v>165</v>
+        <v>184</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="B88" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="C88">
-        <v>2002</v>
+        <v>1954</v>
       </c>
       <c r="D88" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E88" t="s">
-        <v>167</v>
+        <v>185</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B89" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C89">
-        <v>-6000</v>
+        <v>2014</v>
       </c>
       <c r="D89" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="E89" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B90" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C90">
-        <v>-1500</v>
+        <v>2018</v>
       </c>
       <c r="D90" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E90" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="B91" t="s">
-        <v>173</v>
+        <v>68</v>
       </c>
       <c r="C91">
-        <v>-400</v>
+        <v>1983</v>
       </c>
       <c r="D91" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E91" t="s">
-        <v>177</v>
-      </c>
-      <c r="F91" s="4" t="s">
-        <v>178</v>
+        <v>192</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="B92" t="s">
-        <v>173</v>
+        <v>68</v>
       </c>
       <c r="C92">
-        <v>1920</v>
+        <v>1993</v>
       </c>
       <c r="D92" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E92" t="s">
-        <v>179</v>
+        <v>151</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>180</v>
+        <v>152</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="B93" t="s">
-        <v>173</v>
+        <v>68</v>
       </c>
       <c r="C93">
-        <v>1972</v>
+        <v>1993</v>
       </c>
       <c r="D93" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E93" t="s">
-        <v>24</v>
-      </c>
-      <c r="F93" s="4" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="B94" t="s">
-        <v>173</v>
+        <v>68</v>
       </c>
       <c r="C94">
-        <v>1977</v>
+        <v>1993</v>
       </c>
       <c r="D94" t="s">
         <v>10</v>
       </c>
       <c r="E94" t="s">
-        <v>182</v>
-      </c>
-      <c r="F94" s="4" t="s">
-        <v>183</v>
+        <v>153</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="B95" t="s">
-        <v>173</v>
+        <v>68</v>
       </c>
       <c r="C95">
-        <v>1851</v>
+        <v>2011</v>
       </c>
       <c r="D95" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E95" t="s">
-        <v>184</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>185</v>
+        <v>154</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="B96" t="s">
-        <v>173</v>
+        <v>68</v>
       </c>
       <c r="C96">
-        <v>1859</v>
+        <v>1993</v>
       </c>
       <c r="D96" t="s">
         <v>11</v>
       </c>
       <c r="E96" t="s">
-        <v>186</v>
+        <v>156</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="B97" t="s">
-        <v>173</v>
+        <v>68</v>
       </c>
       <c r="C97">
-        <v>1915</v>
+        <v>1995</v>
       </c>
       <c r="D97" t="s">
         <v>11</v>
       </c>
       <c r="E97" t="s">
-        <v>188</v>
-      </c>
-      <c r="F97" s="4" t="s">
-        <v>187</v>
+        <v>158</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="B98" t="s">
-        <v>173</v>
+        <v>68</v>
       </c>
       <c r="C98">
-        <v>1954</v>
+        <v>1993</v>
       </c>
       <c r="D98" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="E98" t="s">
-        <v>189</v>
+        <v>160</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>190</v>
+        <v>161</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="B99" t="s">
-        <v>173</v>
+        <v>68</v>
       </c>
       <c r="C99">
-        <v>2014</v>
+        <v>2021</v>
       </c>
       <c r="D99" t="s">
         <v>33</v>
       </c>
       <c r="E99" t="s">
-        <v>191</v>
+        <v>162</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>192</v>
+        <v>161</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="B100" t="s">
-        <v>173</v>
+        <v>68</v>
       </c>
       <c r="C100">
-        <v>2018</v>
+        <v>2002</v>
       </c>
       <c r="D100" t="s">
         <v>14</v>
       </c>
       <c r="E100" t="s">
-        <v>193</v>
+        <v>163</v>
       </c>
       <c r="F100" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>191</v>
+      </c>
+      <c r="B101" t="s">
+        <v>68</v>
+      </c>
+      <c r="C101">
+        <v>1980</v>
+      </c>
+      <c r="D101" t="s">
+        <v>7</v>
+      </c>
+      <c r="E101" t="s">
         <v>194</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>191</v>
+      </c>
+      <c r="B102" t="s">
+        <v>68</v>
+      </c>
+      <c r="C102">
+        <v>1992</v>
+      </c>
+      <c r="D102" t="s">
+        <v>7</v>
+      </c>
+      <c r="E102" t="s">
+        <v>197</v>
+      </c>
+      <c r="F102" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>191</v>
+      </c>
+      <c r="B103" t="s">
+        <v>68</v>
+      </c>
+      <c r="C103">
+        <v>1997</v>
+      </c>
+      <c r="D103" t="s">
+        <v>7</v>
+      </c>
+      <c r="E103" t="s">
+        <v>198</v>
+      </c>
+      <c r="F103" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>191</v>
+      </c>
+      <c r="B104" t="s">
+        <v>68</v>
+      </c>
+      <c r="C104">
+        <v>1996</v>
+      </c>
+      <c r="D104" t="s">
+        <v>7</v>
+      </c>
+      <c r="E104" t="s">
+        <v>201</v>
+      </c>
+      <c r="F104" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>191</v>
+      </c>
+      <c r="B105" t="s">
+        <v>68</v>
+      </c>
+      <c r="C105">
+        <v>1982</v>
+      </c>
+      <c r="D105" t="s">
+        <v>7</v>
+      </c>
+      <c r="E105" t="s">
+        <v>203</v>
+      </c>
+      <c r="F105" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>191</v>
+      </c>
+      <c r="B106" t="s">
+        <v>68</v>
+      </c>
+      <c r="C106">
+        <v>1986</v>
+      </c>
+      <c r="D106" t="s">
+        <v>7</v>
+      </c>
+      <c r="E106" t="s">
+        <v>204</v>
+      </c>
+      <c r="F106" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -2973,14 +3126,15 @@
     <hyperlink ref="F73" r:id="rId8" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC2366652/" xr:uid="{9DC98DF2-62DB-4FF7-BA05-9727699C3822}"/>
     <hyperlink ref="F75" r:id="rId9" display="https://www.nature.com/articles/srep25280" xr:uid="{B0C93704-3820-4E25-84DD-8FCEFD8C0CD0}"/>
     <hyperlink ref="F76" r:id="rId10" xr:uid="{089EA9DE-A605-4A4F-9C18-13F925DAF593}"/>
-    <hyperlink ref="F83" r:id="rId11" xr:uid="{AAEDCFCB-70FA-4F79-8D1B-F5CB7A1D3BAD}"/>
-    <hyperlink ref="F84" r:id="rId12" xr:uid="{8E682BE9-A46D-41E8-8864-3606AD6E6033}"/>
-    <hyperlink ref="F91" r:id="rId13" xr:uid="{D734C99A-AF20-4CAD-93AF-32A78CF21600}"/>
-    <hyperlink ref="F93" r:id="rId14" xr:uid="{A19BA53C-CA99-4294-B272-3E59309538FE}"/>
-    <hyperlink ref="F94" r:id="rId15" xr:uid="{DA022B77-06BE-4407-ABE8-B9468B1EA7B7}"/>
-    <hyperlink ref="F97" r:id="rId16" xr:uid="{0DBEA179-5D12-4C18-AE5E-1CC00B72C03F}"/>
+    <hyperlink ref="F95" r:id="rId11" xr:uid="{AAEDCFCB-70FA-4F79-8D1B-F5CB7A1D3BAD}"/>
+    <hyperlink ref="F96" r:id="rId12" xr:uid="{8E682BE9-A46D-41E8-8864-3606AD6E6033}"/>
+    <hyperlink ref="F81" r:id="rId13" xr:uid="{D734C99A-AF20-4CAD-93AF-32A78CF21600}"/>
+    <hyperlink ref="F83" r:id="rId14" xr:uid="{A19BA53C-CA99-4294-B272-3E59309538FE}"/>
+    <hyperlink ref="F84" r:id="rId15" xr:uid="{DA022B77-06BE-4407-ABE8-B9468B1EA7B7}"/>
+    <hyperlink ref="F87" r:id="rId16" xr:uid="{0DBEA179-5D12-4C18-AE5E-1CC00B72C03F}"/>
+    <hyperlink ref="F101" r:id="rId17" xr:uid="{0787FCB0-1FE8-4A4A-90D0-F3C3878D224A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>